<commit_message>
Only dashboard module and Update function on Orders missing, plus little extras.
</commit_message>
<xml_diff>
--- a/BORDABLU LIBRO 2021.xlsx
+++ b/BORDABLU LIBRO 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b5ba9e85dce28a7b/Fotos/Vectors/Bordablu/FinanzasApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="8_{5004DFFD-CD1B-40FF-A17C-257C8A3703BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3D1123E-C312-430C-9795-7B5706A342EE}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="8_{5004DFFD-CD1B-40FF-A17C-257C8A3703BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F71FBC69-78B5-48CE-8C3F-73AAE878F31A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{04A73DB8-F961-4374-A989-B7E3F24B30A9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{04A73DB8-F961-4374-A989-B7E3F24B30A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Encargos" sheetId="3" r:id="rId1"/>
@@ -449,10 +449,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2161,8 +2161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C17AA3E-F9A7-4A58-8237-AE75C69B261F}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2171,18 +2171,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="8">
-        <v>50</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2191,7 +2191,7 @@
       </c>
       <c r="B4" s="2">
         <f>B3/1.13</f>
-        <v>44.247787610619476</v>
+        <v>11.061946902654869</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2200,7 +2200,7 @@
       </c>
       <c r="B5" s="2">
         <f>B4*0.04</f>
-        <v>1.7699115044247791</v>
+        <v>0.44247787610619477</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2209,8 +2209,9 @@
       </c>
       <c r="B6" s="2">
         <f>B5*0.13</f>
-        <v>0.23008849557522129</v>
-      </c>
+        <v>5.7522123893805323E-2</v>
+      </c>
+      <c r="C6" s="17"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -2218,7 +2219,7 @@
       </c>
       <c r="B7" s="4">
         <f>B3-(B5+B6)</f>
-        <v>48</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2227,7 +2228,7 @@
       </c>
       <c r="B8" s="6">
         <f>B5+B6</f>
-        <v>2.0000000000000004</v>
+        <v>0.50000000000000011</v>
       </c>
     </row>
   </sheetData>
@@ -2242,7 +2243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB839928-3A9F-486B-8D9A-30D4E62B43BE}">
   <dimension ref="A1:O92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -2263,21 +2264,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>